<commit_message>
Support Vector Machine training implemented
</commit_message>
<xml_diff>
--- a/Configurations/Best.xlsx
+++ b/Configurations/Best.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jorge\Documents\Universidad\Sistemas Inteligentes\Tareas\Classification-Methods\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE62CEA-6CD4-4D99-80D1-5E7394DAB61A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B04F61A-F404-4055-B81E-31EB1E85DA67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38595" yWindow="2775" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38595" yWindow="2775" windowWidth="14400" windowHeight="7365" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CompleteRFC" sheetId="1" r:id="rId1"/>
+    <sheet name="CompleteSVM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Criterion</t>
   </si>
@@ -40,6 +41,21 @@
   </si>
   <si>
     <t>gini</t>
+  </si>
+  <si>
+    <t>Kernel</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>rbf</t>
+  </si>
+  <si>
+    <t>scale</t>
   </si>
 </sst>
 </file>
@@ -369,7 +385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -413,4 +429,41 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9CADA2F-3623-4E78-8B41-B249D9AA60FF}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>1.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
NO and NaN preprocess added
</commit_message>
<xml_diff>
--- a/Configurations/Best.xlsx
+++ b/Configurations/Best.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jorge\Documents\Universidad\Sistemas Inteligentes\Tareas\Classification-Methods\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B04F61A-F404-4055-B81E-31EB1E85DA67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CBCA61-E375-49CC-82A2-B24F1E1669F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38595" yWindow="2775" windowWidth="14400" windowHeight="7365" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -433,15 +433,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9CADA2F-3623-4E78-8B41-B249D9AA60FF}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -452,7 +452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -460,10 +460,14 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>1.9</v>
-      </c>
+        <v>1.9624999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>